<commit_message>
updated pin mappings - changed a bunch for better placements
</commit_message>
<xml_diff>
--- a/Documentation/ESC/pinMapping.xlsx
+++ b/Documentation/ESC/pinMapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prj\qc\Documentation\ESC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF8C5B4-5823-40F3-B3D0-E3D55B3F85C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC0EBE1-278A-4830-9AEC-E29ADE11C714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA712D6F-27C2-4467-A9D7-DE46DEF4EEBD}"/>
   </bookViews>
@@ -1008,8 +1008,8 @@
   </sheetPr>
   <dimension ref="H2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1396,7 @@
         <v>16</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>87</v>
@@ -1452,7 +1452,7 @@
         <v>18</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>89</v>
@@ -1508,7 +1508,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>91</v>
@@ -1564,7 +1564,7 @@
         <v>22</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>93</v>

</xml_diff>